<commit_message>
Add apdate fille userstory.xls
</commit_message>
<xml_diff>
--- a/userstory.xlsx
+++ b/userstory.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="User story" sheetId="1" r:id="rId1"/>
@@ -17,13 +17,14 @@
     <sheet name="Bug report 7" sheetId="8" r:id="rId8"/>
     <sheet name="Bug report 8" sheetId="9" r:id="rId9"/>
     <sheet name="Bug report 9" sheetId="10" r:id="rId10"/>
+    <sheet name="Test Case" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="251">
   <si>
     <t>Коментар</t>
   </si>
@@ -671,9 +672,6 @@
     <t xml:space="preserve">Виконати тестування за чеклистом </t>
   </si>
   <si>
-    <t>Відпраити файл у дириекторію репозеторію</t>
-  </si>
-  <si>
     <t>Завантажити у власний репозиторій на GITHUB</t>
   </si>
   <si>
@@ -764,14 +762,220 @@
     <t xml:space="preserve">Написати коміт </t>
   </si>
   <si>
-    <t>команда GIT commit -m "Addet file ad-hoc.xlsx"</t>
+    <t xml:space="preserve">Завантажити файл у GITHUB </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>команда</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> GIT commit -m "Addet file ad-hoc.xlsx"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>команда</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">    git push https://&lt;GITHUB_ACCESS_TOKEN&gt;@github.com/&lt;GITHUB_USERNAME&gt;/&lt;REPOSITORY_NAME&gt;.git        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;GITHUB_ACCESS_TOKEN&gt;  токен   &lt;GITHUB_USERNAME&gt;   свії юзер нейм    &lt;REPOSITORY_NAME&gt;   свій репозеторій</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Отримати токін </t>
+  </si>
+  <si>
+    <t>виконати за даною інструкцією  https://techglimpse.com/git-push-github-token-based-passwordless/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Відпраити файл у дириекторію репозеторію </t>
+  </si>
+  <si>
+    <t>Test Case ID:</t>
+  </si>
+  <si>
+    <t>Test-7424561</t>
+  </si>
+  <si>
+    <t>Test Case Name:</t>
+  </si>
+  <si>
+    <t>Status:</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>Test Type:</t>
+  </si>
+  <si>
+    <t>Creation Date:</t>
+  </si>
+  <si>
+    <t>//2020</t>
+  </si>
+  <si>
+    <t>Priority:</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Execution Date:</t>
+  </si>
+  <si>
+    <t>Pre-Conditions:</t>
+  </si>
+  <si>
+    <t>Step #</t>
+  </si>
+  <si>
+    <t>Steps:</t>
+  </si>
+  <si>
+    <t>Expected Result</t>
+  </si>
+  <si>
+    <t>Version (Build) #</t>
+  </si>
+  <si>
+    <t>Pass/Fail</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> сайт відкрився.Зїявилась головна сторінка сайту</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Test Data:</t>
+  </si>
+  <si>
+    <t>Attachments:</t>
+  </si>
+  <si>
+    <t>Реєстрація на сайті https://tea-touch.com.ua/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">інтернет-магазин </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> https://tea-touch.com.ua/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Особистий кабінет 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">перехід до особистого кабінету </t>
+  </si>
+  <si>
+    <t xml:space="preserve">натиснути реєстрація </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Відкриваєтьсяособистий кабінет </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Відкривається форма реєстрації </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Поле прийняло наші данні </t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Пароль прийнятий отримана рекомендація до мінімальної кількості символів </t>
+  </si>
+  <si>
+    <t>Ввести ім'я Наг</t>
+  </si>
+  <si>
+    <t>Ввести прізвище Наго</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Введене ім'я з'явилося у полі </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Введене прізвище  з'явилося у полі </t>
+  </si>
+  <si>
+    <t>Ввести номер телефону +480784783214</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Введений номер з'явився у полі </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Обрати країну </t>
+  </si>
+  <si>
+    <t xml:space="preserve">при натисканні на поле зїявляється перелік країн </t>
+  </si>
+  <si>
+    <t>Ввести адресу (будьяка)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">З'являється адреса у полі </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Bug report 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Було проведенно декілька таких спроб зареєструватися на сайті та придбати товар і після таких спроб мені закрили доступ до сайту. З урахуванням завантаженості на роботі трохи часу не вистачело переробляти ще один чек лист іншого сайту тому вирішив лишити як воно є </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -886,8 +1090,31 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -909,8 +1136,20 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD8D8D8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -1027,6 +1266,272 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="thick">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="thick">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="thick">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1035,7 +1540,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1192,29 +1697,149 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="16" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1371,15 +1996,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>104776</xdr:rowOff>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>28576</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>427837</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>66252</xdr:rowOff>
+      <xdr:colOff>437362</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>180552</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1396,7 +2021,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3771900" y="11172826"/>
+          <a:off x="3781425" y="9382126"/>
           <a:ext cx="6304762" cy="3390476"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1409,15 +2034,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
+      <xdr:colOff>581025</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>180974</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>4591051</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>9526</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1434,8 +2059,51 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4276725" y="9686925"/>
-          <a:ext cx="4086226" cy="1323975"/>
+          <a:off x="4352925" y="7724774"/>
+          <a:ext cx="4086226" cy="1476375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>267051</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>2548</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Рисунок 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="876651" y="10553700"/>
+          <a:ext cx="15108847" cy="8267700"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1734,11 +2402,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:H88"/>
+  <dimension ref="B4:H89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="C88" sqref="C88"/>
-    </sheetView>
+    <sheetView topLeftCell="A34" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2689,7 +3355,7 @@
     </row>
     <row r="80" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B80" s="40" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C80" s="41"/>
       <c r="D80" s="41"/>
@@ -2700,7 +3366,7 @@
         <v>1</v>
       </c>
       <c r="C81" s="11" t="s">
-        <v>190</v>
+        <v>205</v>
       </c>
       <c r="D81" s="4" t="s">
         <v>1</v>
@@ -2709,10 +3375,10 @@
     </row>
     <row r="82" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B82" s="10">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C82" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D82" s="4" t="s">
         <v>1</v>
@@ -2721,77 +3387,100 @@
     </row>
     <row r="83" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B83" s="10">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C83" s="11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D83" s="4" t="s">
         <v>1</v>
       </c>
       <c r="E83" s="39" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="84" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B84" s="10">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C84" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D84" s="4" t="s">
         <v>1</v>
       </c>
       <c r="E84" s="39" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="85" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B85" s="10">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C85" s="11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D85" s="4" t="s">
         <v>1</v>
       </c>
       <c r="E85" s="39" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="86" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B86" s="10">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C86" s="11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D86" s="4" t="s">
         <v>1</v>
       </c>
       <c r="E86" s="39" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="87" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B87" s="10">
+        <v>7</v>
+      </c>
+      <c r="C87" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="D87" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E87" s="39" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="88" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B88" s="10">
+        <v>8</v>
+      </c>
+      <c r="C88" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="D88" s="63" t="s">
+        <v>1</v>
+      </c>
+      <c r="E88" s="29" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="89" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="B89" s="10">
         <v>9</v>
       </c>
-      <c r="C87" s="11" t="s">
+      <c r="C89" s="64" t="s">
         <v>200</v>
       </c>
-      <c r="D87" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E87" s="2" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B88" s="63">
-        <v>10</v>
+      <c r="D89" s="63" t="s">
+        <v>1</v>
+      </c>
+      <c r="E89" s="65" t="s">
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -2825,7 +3514,7 @@
   <dimension ref="B3:F28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:F4"/>
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2847,16 +3536,16 @@
       <c r="C4" s="21" t="s">
         <v>176</v>
       </c>
-      <c r="E4" s="58" t="s">
+      <c r="E4" s="56" t="s">
         <v>186</v>
       </c>
-      <c r="F4" s="58"/>
+      <c r="F4" s="56"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="C5" s="56" t="s">
+      <c r="C5" s="59" t="s">
         <v>87</v>
       </c>
     </row>
@@ -2921,10 +3610,10 @@
       </c>
     </row>
     <row r="14" spans="2:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="57" t="s">
+      <c r="B14" s="60" t="s">
         <v>101</v>
       </c>
-      <c r="C14" s="57"/>
+      <c r="C14" s="60"/>
     </row>
     <row r="15" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="21" t="s">
@@ -2943,16 +3632,16 @@
       </c>
     </row>
     <row r="17" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="57" t="s">
+      <c r="B17" s="60" t="s">
         <v>106</v>
       </c>
-      <c r="C17" s="57"/>
+      <c r="C17" s="60"/>
     </row>
     <row r="18" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B18" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="C18" s="59" t="s">
+      <c r="C18" s="57" t="s">
         <v>181</v>
       </c>
     </row>
@@ -2960,7 +3649,7 @@
       <c r="B19" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="C19" s="60"/>
+      <c r="C19" s="58"/>
     </row>
     <row r="20" spans="2:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="21">
@@ -3026,17 +3715,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B17:C17"/>
     <mergeCell ref="C22:C23"/>
     <mergeCell ref="C24:C25"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="C27:C28"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="C18:C19"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B17:C17"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C5" r:id="rId1"/>
@@ -3044,6 +3733,373 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:G27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B31" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="35.5703125" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="4" max="4" width="38.140625" customWidth="1"/>
+    <col min="5" max="5" width="39" customWidth="1"/>
+    <col min="7" max="7" width="59.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="66" t="s">
+        <v>206</v>
+      </c>
+      <c r="C5" s="67" t="s">
+        <v>207</v>
+      </c>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="68"/>
+      <c r="G5" s="69"/>
+    </row>
+    <row r="6" spans="2:7" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="70" t="s">
+        <v>208</v>
+      </c>
+      <c r="C6" s="71" t="s">
+        <v>228</v>
+      </c>
+      <c r="D6" s="72"/>
+      <c r="E6" s="72"/>
+      <c r="F6" s="72"/>
+      <c r="G6" s="73"/>
+    </row>
+    <row r="7" spans="2:7" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="70" t="s">
+        <v>209</v>
+      </c>
+      <c r="C7" s="74" t="s">
+        <v>210</v>
+      </c>
+      <c r="D7" s="75"/>
+      <c r="E7" s="75"/>
+      <c r="F7" s="75"/>
+      <c r="G7" s="76"/>
+    </row>
+    <row r="8" spans="2:7" ht="20.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="70" t="s">
+        <v>211</v>
+      </c>
+      <c r="C8" s="74" t="s">
+        <v>229</v>
+      </c>
+      <c r="D8" s="75"/>
+      <c r="E8" s="75"/>
+      <c r="F8" s="75"/>
+      <c r="G8" s="76"/>
+    </row>
+    <row r="9" spans="2:7" ht="23.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="70" t="s">
+        <v>212</v>
+      </c>
+      <c r="C9" s="74" t="s">
+        <v>213</v>
+      </c>
+      <c r="D9" s="75"/>
+      <c r="E9" s="75"/>
+      <c r="F9" s="75"/>
+      <c r="G9" s="76"/>
+    </row>
+    <row r="10" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="70" t="s">
+        <v>214</v>
+      </c>
+      <c r="C10" s="74" t="s">
+        <v>215</v>
+      </c>
+      <c r="D10" s="75"/>
+      <c r="E10" s="75"/>
+      <c r="F10" s="75"/>
+      <c r="G10" s="76"/>
+    </row>
+    <row r="11" spans="2:7" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="77" t="s">
+        <v>216</v>
+      </c>
+      <c r="C11" s="78" t="s">
+        <v>213</v>
+      </c>
+      <c r="D11" s="79"/>
+      <c r="E11" s="79"/>
+      <c r="F11" s="79"/>
+      <c r="G11" s="80"/>
+    </row>
+    <row r="12" spans="2:7" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="81" t="s">
+        <v>217</v>
+      </c>
+      <c r="C12" s="81" t="s">
+        <v>218</v>
+      </c>
+      <c r="D12" s="81" t="s">
+        <v>219</v>
+      </c>
+      <c r="E12" s="81" t="s">
+        <v>220</v>
+      </c>
+      <c r="F12" s="82" t="s">
+        <v>221</v>
+      </c>
+      <c r="G12" s="83"/>
+    </row>
+    <row r="13" spans="2:7" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="84"/>
+      <c r="C13" s="84"/>
+      <c r="D13" s="84"/>
+      <c r="E13" s="84"/>
+      <c r="F13" s="85" t="s">
+        <v>222</v>
+      </c>
+      <c r="G13" s="85" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="47.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="86" t="s">
+        <v>230</v>
+      </c>
+      <c r="C14" s="87">
+        <v>1</v>
+      </c>
+      <c r="D14" s="100" t="s">
+        <v>230</v>
+      </c>
+      <c r="E14" s="88" t="s">
+        <v>224</v>
+      </c>
+      <c r="F14" s="89" t="s">
+        <v>225</v>
+      </c>
+      <c r="G14" s="88"/>
+    </row>
+    <row r="15" spans="2:7" ht="47.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="90" t="s">
+        <v>232</v>
+      </c>
+      <c r="C15" s="87">
+        <v>2</v>
+      </c>
+      <c r="D15" s="101" t="s">
+        <v>231</v>
+      </c>
+      <c r="E15" s="88" t="s">
+        <v>234</v>
+      </c>
+      <c r="F15" s="89" t="s">
+        <v>225</v>
+      </c>
+      <c r="G15" s="88"/>
+    </row>
+    <row r="16" spans="2:7" ht="47.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="90" t="s">
+        <v>160</v>
+      </c>
+      <c r="C16" s="87">
+        <v>3</v>
+      </c>
+      <c r="D16" s="102" t="s">
+        <v>233</v>
+      </c>
+      <c r="E16" s="98" t="s">
+        <v>235</v>
+      </c>
+      <c r="F16" s="89" t="s">
+        <v>225</v>
+      </c>
+      <c r="G16" s="88"/>
+    </row>
+    <row r="17" spans="2:7" ht="47.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="90"/>
+      <c r="C17" s="97">
+        <v>4</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>164</v>
+      </c>
+      <c r="E17" s="26" t="s">
+        <v>236</v>
+      </c>
+      <c r="F17" s="89" t="s">
+        <v>225</v>
+      </c>
+      <c r="G17" s="88" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="47.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="90"/>
+      <c r="C18" s="87">
+        <v>5</v>
+      </c>
+      <c r="D18" s="103" t="s">
+        <v>165</v>
+      </c>
+      <c r="E18" s="99" t="s">
+        <v>238</v>
+      </c>
+      <c r="F18" s="89" t="s">
+        <v>225</v>
+      </c>
+      <c r="G18" s="88" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" ht="47.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="90"/>
+      <c r="C19" s="87">
+        <v>6</v>
+      </c>
+      <c r="D19" s="88" t="s">
+        <v>239</v>
+      </c>
+      <c r="E19" s="88" t="s">
+        <v>241</v>
+      </c>
+      <c r="F19" s="89" t="s">
+        <v>225</v>
+      </c>
+      <c r="G19" s="88" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" ht="47.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="90"/>
+      <c r="C20" s="87">
+        <v>7</v>
+      </c>
+      <c r="D20" s="88" t="s">
+        <v>240</v>
+      </c>
+      <c r="E20" s="88" t="s">
+        <v>242</v>
+      </c>
+      <c r="F20" s="89" t="s">
+        <v>225</v>
+      </c>
+      <c r="G20" s="88" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" ht="47.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="90"/>
+      <c r="C21" s="87">
+        <v>8</v>
+      </c>
+      <c r="D21" s="88" t="s">
+        <v>243</v>
+      </c>
+      <c r="E21" s="88" t="s">
+        <v>244</v>
+      </c>
+      <c r="F21" s="89" t="s">
+        <v>225</v>
+      </c>
+      <c r="G21" s="88" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" ht="47.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="90"/>
+      <c r="C22" s="87">
+        <v>9</v>
+      </c>
+      <c r="D22" s="88" t="s">
+        <v>245</v>
+      </c>
+      <c r="E22" s="88" t="s">
+        <v>246</v>
+      </c>
+      <c r="F22" s="96" t="s">
+        <v>237</v>
+      </c>
+      <c r="G22" s="88" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" ht="47.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="90"/>
+      <c r="C23" s="87">
+        <v>10</v>
+      </c>
+      <c r="D23" s="88" t="s">
+        <v>247</v>
+      </c>
+      <c r="E23" s="88" t="s">
+        <v>248</v>
+      </c>
+      <c r="F23" s="89" t="s">
+        <v>225</v>
+      </c>
+      <c r="G23" s="88"/>
+    </row>
+    <row r="24" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="90"/>
+      <c r="C24" s="87"/>
+      <c r="D24" s="88"/>
+      <c r="E24" s="88"/>
+      <c r="F24" s="89" t="s">
+        <v>225</v>
+      </c>
+      <c r="G24" s="88"/>
+    </row>
+    <row r="25" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="91" t="s">
+        <v>226</v>
+      </c>
+      <c r="C25" s="92">
+        <v>45068</v>
+      </c>
+      <c r="D25" s="93"/>
+      <c r="E25" s="93"/>
+      <c r="F25" s="93"/>
+      <c r="G25" s="94"/>
+    </row>
+    <row r="26" spans="2:7" ht="61.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="91" t="s">
+        <v>227</v>
+      </c>
+      <c r="C26" s="95" t="s">
+        <v>250</v>
+      </c>
+      <c r="D26" s="93"/>
+      <c r="E26" s="93"/>
+      <c r="F26" s="93"/>
+      <c r="G26" s="94"/>
+    </row>
+    <row r="27" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3074,10 +4130,10 @@
       <c r="C4" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="E4" s="58" t="s">
+      <c r="E4" s="56" t="s">
         <v>186</v>
       </c>
-      <c r="F4" s="58"/>
+      <c r="F4" s="56"/>
       <c r="G4" s="28"/>
       <c r="H4" s="28"/>
     </row>
@@ -3085,7 +4141,7 @@
       <c r="B5" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="C5" s="56" t="s">
+      <c r="C5" s="59" t="s">
         <v>123</v>
       </c>
     </row>
@@ -3150,10 +4206,10 @@
       </c>
     </row>
     <row r="14" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="57" t="s">
+      <c r="B14" s="60" t="s">
         <v>101</v>
       </c>
-      <c r="C14" s="57"/>
+      <c r="C14" s="60"/>
     </row>
     <row r="15" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B15" s="21" t="s">
@@ -3172,16 +4228,16 @@
       </c>
     </row>
     <row r="17" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="57" t="s">
+      <c r="B17" s="60" t="s">
         <v>106</v>
       </c>
-      <c r="C17" s="57"/>
+      <c r="C17" s="60"/>
     </row>
     <row r="18" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B18" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="C18" s="59" t="s">
+      <c r="C18" s="57" t="s">
         <v>122</v>
       </c>
     </row>
@@ -3189,7 +4245,7 @@
       <c r="B19" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="C19" s="60"/>
+      <c r="C19" s="58"/>
     </row>
     <row r="20" spans="2:3" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="21">
@@ -3279,17 +4335,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B17:C17"/>
     <mergeCell ref="C25:C26"/>
     <mergeCell ref="C27:C28"/>
     <mergeCell ref="B29:C29"/>
     <mergeCell ref="C30:C31"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="C18:C19"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B17:C17"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C5" r:id="rId1"/>
@@ -3327,16 +4383,16 @@
       <c r="C4" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="E4" s="58" t="s">
+      <c r="E4" s="56" t="s">
         <v>186</v>
       </c>
-      <c r="F4" s="58"/>
+      <c r="F4" s="56"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="C5" s="56" t="s">
+      <c r="C5" s="59" t="s">
         <v>123</v>
       </c>
     </row>
@@ -3401,10 +4457,10 @@
       </c>
     </row>
     <row r="14" spans="2:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="57" t="s">
+      <c r="B14" s="60" t="s">
         <v>101</v>
       </c>
-      <c r="C14" s="57"/>
+      <c r="C14" s="60"/>
     </row>
     <row r="15" spans="2:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="21" t="s">
@@ -3423,16 +4479,16 @@
       </c>
     </row>
     <row r="17" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="57" t="s">
+      <c r="B17" s="60" t="s">
         <v>106</v>
       </c>
-      <c r="C17" s="57"/>
+      <c r="C17" s="60"/>
     </row>
     <row r="18" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B18" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="C18" s="59" t="s">
+      <c r="C18" s="57" t="s">
         <v>122</v>
       </c>
     </row>
@@ -3440,7 +4496,7 @@
       <c r="B19" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="C19" s="60"/>
+      <c r="C19" s="58"/>
     </row>
     <row r="20" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B20" s="21">
@@ -3522,17 +4578,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B17:C17"/>
     <mergeCell ref="C24:C25"/>
     <mergeCell ref="C26:C27"/>
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="C29:C30"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="C18:C19"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B17:C17"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C5" r:id="rId1"/>
@@ -3570,16 +4626,16 @@
       <c r="C3" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="E3" s="58" t="s">
+      <c r="E3" s="56" t="s">
         <v>186</v>
       </c>
-      <c r="F3" s="58"/>
+      <c r="F3" s="56"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="C4" s="56" t="s">
+      <c r="C4" s="59" t="s">
         <v>123</v>
       </c>
     </row>
@@ -3644,10 +4700,10 @@
       </c>
     </row>
     <row r="13" spans="2:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="57" t="s">
+      <c r="B13" s="60" t="s">
         <v>101</v>
       </c>
-      <c r="C13" s="57"/>
+      <c r="C13" s="60"/>
     </row>
     <row r="14" spans="2:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="21" t="s">
@@ -3666,16 +4722,16 @@
       </c>
     </row>
     <row r="16" spans="2:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="57" t="s">
+      <c r="B16" s="60" t="s">
         <v>106</v>
       </c>
-      <c r="C16" s="57"/>
+      <c r="C16" s="60"/>
     </row>
     <row r="17" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B17" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="C17" s="59" t="s">
+      <c r="C17" s="57" t="s">
         <v>122</v>
       </c>
     </row>
@@ -3683,7 +4739,7 @@
       <c r="B18" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="C18" s="60"/>
+      <c r="C18" s="58"/>
     </row>
     <row r="19" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B19" s="21">
@@ -3765,17 +4821,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B16:C16"/>
     <mergeCell ref="C23:C24"/>
     <mergeCell ref="C25:C26"/>
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="C28:C29"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="C17:C18"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B16:C16"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1"/>
@@ -3812,16 +4868,16 @@
       <c r="C4" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="E4" s="58" t="s">
+      <c r="E4" s="56" t="s">
         <v>186</v>
       </c>
-      <c r="F4" s="58"/>
+      <c r="F4" s="56"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="C5" s="56" t="s">
+      <c r="C5" s="59" t="s">
         <v>123</v>
       </c>
     </row>
@@ -3886,10 +4942,10 @@
       </c>
     </row>
     <row r="14" spans="2:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="57" t="s">
+      <c r="B14" s="60" t="s">
         <v>101</v>
       </c>
-      <c r="C14" s="57"/>
+      <c r="C14" s="60"/>
     </row>
     <row r="15" spans="2:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="21" t="s">
@@ -3908,16 +4964,16 @@
       </c>
     </row>
     <row r="17" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="57" t="s">
+      <c r="B17" s="60" t="s">
         <v>106</v>
       </c>
-      <c r="C17" s="57"/>
+      <c r="C17" s="60"/>
     </row>
     <row r="18" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B18" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="C18" s="59" t="s">
+      <c r="C18" s="57" t="s">
         <v>122</v>
       </c>
     </row>
@@ -3925,7 +4981,7 @@
       <c r="B19" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="C19" s="60"/>
+      <c r="C19" s="58"/>
     </row>
     <row r="20" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B20" s="21">
@@ -4007,17 +5063,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B17:C17"/>
     <mergeCell ref="C24:C25"/>
     <mergeCell ref="C26:C27"/>
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="C29:C30"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="C18:C19"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B17:C17"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C5" r:id="rId1"/>
@@ -4031,7 +5087,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="E3" sqref="E3:F3"/>
     </sheetView>
   </sheetViews>
@@ -4057,13 +5113,13 @@
       <c r="E3" s="61" t="s">
         <v>186</v>
       </c>
-      <c r="F3" s="58"/>
+      <c r="F3" s="56"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="C4" s="56" t="s">
+      <c r="C4" s="59" t="s">
         <v>87</v>
       </c>
     </row>
@@ -4128,10 +5184,10 @@
       </c>
     </row>
     <row r="13" spans="2:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="57" t="s">
+      <c r="B13" s="60" t="s">
         <v>101</v>
       </c>
-      <c r="C13" s="57"/>
+      <c r="C13" s="60"/>
     </row>
     <row r="14" spans="2:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="21" t="s">
@@ -4150,16 +5206,16 @@
       </c>
     </row>
     <row r="16" spans="2:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="57" t="s">
+      <c r="B16" s="60" t="s">
         <v>106</v>
       </c>
-      <c r="C16" s="57"/>
+      <c r="C16" s="60"/>
     </row>
     <row r="17" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B17" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="C17" s="59" t="s">
+      <c r="C17" s="57" t="s">
         <v>108</v>
       </c>
     </row>
@@ -4167,7 +5223,7 @@
       <c r="B18" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="C18" s="60"/>
+      <c r="C18" s="58"/>
     </row>
     <row r="19" spans="2:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="21">
@@ -4249,17 +5305,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B16:C16"/>
     <mergeCell ref="C23:C24"/>
     <mergeCell ref="C25:C26"/>
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="C28:C29"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="C17:C18"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B16:C16"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1"/>
@@ -4274,7 +5330,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:F32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="E4" sqref="E4:F4"/>
     </sheetView>
   </sheetViews>
@@ -4297,16 +5353,16 @@
       <c r="C4" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="E4" s="58" t="s">
+      <c r="E4" s="56" t="s">
         <v>186</v>
       </c>
-      <c r="F4" s="58"/>
+      <c r="F4" s="56"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="C5" s="56" t="s">
+      <c r="C5" s="59" t="s">
         <v>87</v>
       </c>
     </row>
@@ -4371,10 +5427,10 @@
       </c>
     </row>
     <row r="14" spans="2:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="57" t="s">
+      <c r="B14" s="60" t="s">
         <v>101</v>
       </c>
-      <c r="C14" s="57"/>
+      <c r="C14" s="60"/>
     </row>
     <row r="15" spans="2:6" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="21" t="s">
@@ -4393,16 +5449,16 @@
       </c>
     </row>
     <row r="17" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="57" t="s">
+      <c r="B17" s="60" t="s">
         <v>106</v>
       </c>
-      <c r="C17" s="57"/>
+      <c r="C17" s="60"/>
     </row>
     <row r="18" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B18" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="C18" s="59" t="s">
+      <c r="C18" s="57" t="s">
         <v>140</v>
       </c>
     </row>
@@ -4410,7 +5466,7 @@
       <c r="B19" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="C19" s="60"/>
+      <c r="C19" s="58"/>
     </row>
     <row r="20" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B20" s="21">
@@ -4508,17 +5564,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B17:C17"/>
     <mergeCell ref="C26:C27"/>
     <mergeCell ref="C28:C29"/>
     <mergeCell ref="B30:C30"/>
     <mergeCell ref="C31:C32"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="C18:C19"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B17:C17"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C5" r:id="rId1"/>
@@ -4533,7 +5589,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:F30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="E4" sqref="E4:F4"/>
     </sheetView>
   </sheetViews>
@@ -4556,16 +5612,16 @@
       <c r="C4" s="21" t="s">
         <v>151</v>
       </c>
-      <c r="E4" s="58" t="s">
+      <c r="E4" s="56" t="s">
         <v>186</v>
       </c>
-      <c r="F4" s="58"/>
+      <c r="F4" s="56"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="C5" s="56" t="s">
+      <c r="C5" s="59" t="s">
         <v>87</v>
       </c>
     </row>
@@ -4630,10 +5686,10 @@
       </c>
     </row>
     <row r="14" spans="2:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="57" t="s">
+      <c r="B14" s="60" t="s">
         <v>101</v>
       </c>
-      <c r="C14" s="57"/>
+      <c r="C14" s="60"/>
     </row>
     <row r="15" spans="2:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="21" t="s">
@@ -4652,16 +5708,16 @@
       </c>
     </row>
     <row r="17" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="57" t="s">
+      <c r="B17" s="60" t="s">
         <v>106</v>
       </c>
-      <c r="C17" s="57"/>
+      <c r="C17" s="60"/>
     </row>
     <row r="18" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B18" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="C18" s="59" t="s">
+      <c r="C18" s="57" t="s">
         <v>153</v>
       </c>
     </row>
@@ -4669,7 +5725,7 @@
       <c r="B19" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="C19" s="60"/>
+      <c r="C19" s="58"/>
     </row>
     <row r="20" spans="2:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="21">
@@ -4751,17 +5807,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B17:C17"/>
     <mergeCell ref="C24:C25"/>
     <mergeCell ref="C26:C27"/>
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="C29:C30"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="C18:C19"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B17:C17"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C5" r:id="rId1"/>
@@ -4775,8 +5831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:F37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:F4"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4798,16 +5854,16 @@
       <c r="C4" s="21" t="s">
         <v>160</v>
       </c>
-      <c r="E4" s="58" t="s">
+      <c r="E4" s="56" t="s">
         <v>186</v>
       </c>
-      <c r="F4" s="58"/>
+      <c r="F4" s="56"/>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="C5" s="56" t="s">
+      <c r="C5" s="59" t="s">
         <v>87</v>
       </c>
     </row>
@@ -4872,10 +5928,10 @@
       </c>
     </row>
     <row r="14" spans="2:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="57" t="s">
+      <c r="B14" s="60" t="s">
         <v>101</v>
       </c>
-      <c r="C14" s="57"/>
+      <c r="C14" s="60"/>
     </row>
     <row r="15" spans="2:6" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="21" t="s">
@@ -4894,16 +5950,16 @@
       </c>
     </row>
     <row r="17" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="57" t="s">
+      <c r="B17" s="60" t="s">
         <v>106</v>
       </c>
-      <c r="C17" s="57"/>
+      <c r="C17" s="60"/>
     </row>
     <row r="18" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B18" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="C18" s="59" t="s">
+      <c r="C18" s="57" t="s">
         <v>163</v>
       </c>
     </row>
@@ -4911,7 +5967,7 @@
       <c r="B19" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="C19" s="60"/>
+      <c r="C19" s="58"/>
     </row>
     <row r="20" spans="2:3" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="21">
@@ -5049,17 +6105,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B17:C17"/>
     <mergeCell ref="C31:C32"/>
     <mergeCell ref="C33:C34"/>
     <mergeCell ref="B35:C35"/>
     <mergeCell ref="C36:C37"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="C18:C19"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B17:C17"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C5" r:id="rId1"/>

</xml_diff>